<commit_message>
Include diavolezza drone points
</commit_message>
<xml_diff>
--- a/data/gangles21/raw/Gangles Data - Surya.xlsx
+++ b/data/gangles21/raw/Gangles Data - Surya.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
   <si>
     <t xml:space="preserve">Gangles Ice Stupa 2020-21 season timeline </t>
   </si>
@@ -31,6 +31,9 @@
     <t xml:space="preserve">Activity</t>
   </si>
   <si>
+    <t xml:space="preserve">Questions</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dome 1 making start</t>
   </si>
   <si>
@@ -64,6 +67,9 @@
     <t xml:space="preserve">Water frozen, pipe cleared, dome 2 completed, started water via dome 2 at 4.30 PM through vaccume pipe</t>
   </si>
   <si>
+    <t xml:space="preserve">Fountain height: 5 m?(2 GI pipes of 6 ft)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Water running, dome 2 collapsed &amp; remade by added umbu and started water at 4.30 PM</t>
   </si>
   <si>
@@ -71,6 +77,9 @@
   </si>
   <si>
     <t xml:space="preserve">Water running, added GI pipe &amp; umbu and started water at 5 PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fountain height: 9 m? (4 GI pipes of 6 ft)</t>
   </si>
   <si>
     <t xml:space="preserve">Water running, added umbu and started water at 5 PM</t>
@@ -114,7 +123,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -144,6 +153,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -211,7 +226,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -244,7 +259,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -331,14 +350,15 @@
   </sheetPr>
   <dimension ref="A1:L87"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C30" activeCellId="0" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="42.91"/>
   </cols>
   <sheetData>
@@ -357,6 +377,9 @@
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="C2" s="0" t="s">
+        <v>3</v>
+      </c>
       <c r="K2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -364,7 +387,7 @@
         <v>44191</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K3" s="3"/>
     </row>
@@ -373,7 +396,7 @@
         <v>44192</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K4" s="3"/>
     </row>
@@ -390,7 +413,7 @@
         <v>44194</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K6" s="3"/>
       <c r="L6" s="6"/>
@@ -400,7 +423,7 @@
         <v>44195</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K7" s="3"/>
       <c r="L7" s="6"/>
@@ -410,7 +433,7 @@
         <v>44196</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K8" s="3"/>
     </row>
@@ -434,7 +457,7 @@
         <v>44199</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K11" s="3"/>
       <c r="L11" s="6"/>
@@ -444,7 +467,7 @@
         <v>44200</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K12" s="3"/>
       <c r="L12" s="6"/>
@@ -454,7 +477,7 @@
         <v>44201</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K13" s="3"/>
       <c r="L13" s="6"/>
@@ -472,7 +495,7 @@
         <v>44203</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K15" s="3"/>
       <c r="L15" s="6"/>
@@ -490,7 +513,7 @@
         <v>44205</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K17" s="3"/>
       <c r="L17" s="6"/>
@@ -516,7 +539,7 @@
         <v>44208</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K20" s="3"/>
       <c r="L20" s="6"/>
@@ -542,7 +565,7 @@
         <v>44211</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K23" s="3"/>
       <c r="L23" s="6"/>
@@ -563,12 +586,15 @@
       <c r="K25" s="3"/>
       <c r="L25" s="6"/>
     </row>
-    <row r="26" customFormat="false" ht="41.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="n">
         <v>44214</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="K26" s="3"/>
       <c r="L26" s="6"/>
@@ -578,7 +604,7 @@
         <v>44215</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="K27" s="3"/>
       <c r="L27" s="6"/>
@@ -596,7 +622,7 @@
         <v>44217</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K29" s="3"/>
       <c r="L29" s="6"/>
@@ -605,8 +631,11 @@
       <c r="A30" s="4" t="n">
         <v>44218</v>
       </c>
-      <c r="B30" s="8" t="s">
-        <v>16</v>
+      <c r="B30" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="K30" s="3"/>
       <c r="L30" s="6"/>
@@ -616,7 +645,7 @@
         <v>44219</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="K31" s="3"/>
       <c r="L31" s="6"/>
@@ -626,7 +655,7 @@
         <v>44220</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="K32" s="3"/>
       <c r="L32" s="6"/>
@@ -668,7 +697,7 @@
         <v>44225</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="K37" s="3"/>
       <c r="L37" s="6"/>
@@ -678,7 +707,7 @@
         <v>44226</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="K38" s="3"/>
       <c r="L38" s="6"/>
@@ -688,7 +717,7 @@
         <v>44227</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="K39" s="3"/>
       <c r="L39" s="6"/>
@@ -706,7 +735,7 @@
         <v>44229</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="K41" s="3"/>
       <c r="L41" s="6"/>
@@ -748,7 +777,7 @@
         <v>44234</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="K46" s="3"/>
       <c r="L46" s="6"/>
@@ -766,7 +795,7 @@
         <v>44236</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="K48" s="3"/>
       <c r="L48" s="6"/>
@@ -800,7 +829,7 @@
         <v>44240</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="K52" s="3"/>
       <c r="L52" s="6"/>
@@ -810,7 +839,7 @@
         <v>44241</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="K53" s="3"/>
       <c r="L53" s="6"/>
@@ -820,7 +849,7 @@
         <v>44242</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="K54" s="3"/>
       <c r="L54" s="6"/>
@@ -854,7 +883,7 @@
         <v>44246</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="K58" s="3"/>
       <c r="L58" s="6"/>
@@ -880,7 +909,7 @@
         <v>44249</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="K61" s="3"/>
       <c r="L61" s="6"/>
@@ -898,7 +927,7 @@
         <v>44251</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="K63" s="3"/>
       <c r="L63" s="6"/>
@@ -924,7 +953,7 @@
         <v>44254</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="K66" s="3"/>
       <c r="L66" s="6"/>
@@ -958,7 +987,7 @@
         <v>44258</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="K70" s="3"/>
       <c r="L70" s="6"/>
@@ -976,7 +1005,7 @@
         <v>44260</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="K72" s="3"/>
       <c r="L72" s="6"/>
@@ -986,7 +1015,7 @@
         <v>44261</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="K73" s="3"/>
       <c r="L73" s="6"/>
@@ -996,7 +1025,7 @@
         <v>44262</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="K74" s="3"/>
       <c r="L74" s="6"/>
@@ -1006,7 +1035,7 @@
         <v>44263</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="K75" s="3"/>
       <c r="L75" s="6"/>
@@ -1016,7 +1045,7 @@
         <v>44264</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="K76" s="3"/>
       <c r="L76" s="6"/>
@@ -1026,11 +1055,11 @@
         <v>44265</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="9"/>
+      <c r="A78" s="10"/>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="3"/>

</xml_diff>